<commit_message>
Changes related to manuscript preparation and compatibility and development of SegmentImage.mlapp
</commit_message>
<xml_diff>
--- a/Data/P0/P0_SupportCells_SegSchedule.xlsx
+++ b/Data/P0/P0_SupportCells_SegSchedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Box Sync\Research\Projects\Vestibular Hair Cell Analysis\Ear-Cell-Analysis-Code\Data\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABEE028-DE26-418D-A6B8-C5763B4365C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F995D93A-8F90-41CF-8B03-9447B33EF445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="0" windowWidth="18495" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,9 +146,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +442,7 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -457,7 +458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -465,7 +466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -476,7 +477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -487,7 +488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -495,7 +496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -503,7 +504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -511,7 +512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -525,7 +526,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -533,25 +534,28 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -559,7 +563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -567,16 +571,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>200</v>
       </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">

</xml_diff>